<commit_message>
added HTA and diabetes
</commit_message>
<xml_diff>
--- a/input/STEPS_Instrument_V3_2_2_V3.xlsx
+++ b/input/STEPS_Instrument_V3_2_2_V3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1937,7 +1937,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4484,7 +4484,7 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D48" sqref="D48:E48"/>
     </sheetView>
   </sheetViews>

</xml_diff>